<commit_message>
docs: deliverables final version
</commit_message>
<xml_diff>
--- a/docs/Sprint 0/deliverables/10-DP-dedication.xlsx
+++ b/docs/Sprint 0/deliverables/10-DP-dedication.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29721"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santi\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{FCEE317E-BB54-4E85-9248-14271C57C98C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4DD26575-9C0F-41C5-AF09-35A65E2D1C91}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06ABD54B-6159-44ED-B6A0-572BCC867DA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{02C8C9D8-2F21-45BA-9A66-91BB45160C54}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="56">
   <si>
     <t>Nombre</t>
   </si>
@@ -206,13 +206,16 @@
   </si>
   <si>
     <t>Comentarios sobre DP</t>
+  </si>
+  <si>
+    <t>Manuel Chica Lopez se incorporó mas tarde en el grupo, por esto tiene menos horas en Clockify</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,6 +266,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -272,7 +290,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -295,12 +313,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -332,6 +359,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -758,18 +795,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30DF89C9-C95E-4402-8344-C5801FC30A20}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
-    <col min="2" max="2" width="38.140625" customWidth="1"/>
-    <col min="3" max="7" width="10.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="16.1796875" customWidth="1"/>
+    <col min="2" max="2" width="38.1796875" customWidth="1"/>
+    <col min="3" max="7" width="10.7265625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="5" customFormat="1" ht="42.75" thickBot="1">
+    <row r="1" spans="1:7" s="5" customFormat="1" ht="46.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -792,7 +829,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1">
+    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -800,14 +837,14 @@
         <v>8</v>
       </c>
       <c r="C2" s="3">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" ht="30" customHeight="1" thickBot="1">
+    <row r="3" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -822,7 +859,7 @@
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:7" ht="25.5" thickBot="1">
+    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -837,7 +874,7 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1">
+    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -845,14 +882,14 @@
         <v>13</v>
       </c>
       <c r="C5" s="3">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -867,7 +904,7 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7" ht="25.5" thickBot="1">
+    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -882,11 +919,11 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" thickBot="1">
+    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="15" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="3">
@@ -897,7 +934,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" thickBot="1">
+    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -912,7 +949,7 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" thickBot="1">
+    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
@@ -927,7 +964,7 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:7" ht="25.5" thickBot="1">
+    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
@@ -942,7 +979,7 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" thickBot="1">
+    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
@@ -957,7 +994,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" thickBot="1">
+    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
@@ -972,7 +1009,7 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
@@ -987,7 +1024,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>32</v>
       </c>
@@ -1002,7 +1039,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" thickBot="1">
+    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
@@ -1017,7 +1054,7 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:7" ht="25.5" thickBot="1">
+    <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
         <v>35</v>
       </c>
@@ -1032,7 +1069,7 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="1:7" ht="15.75" thickBot="1">
+    <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
         <v>37</v>
       </c>
@@ -1047,7 +1084,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:7" ht="15.75" thickBot="1">
+    <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
         <v>39</v>
       </c>
@@ -1062,7 +1099,7 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="1:7" ht="15.75" thickBot="1">
+    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
         <v>41</v>
       </c>
@@ -1077,7 +1114,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:7" ht="15.75" thickBot="1">
+    <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
         <v>37</v>
       </c>
@@ -1092,7 +1129,7 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>44</v>
       </c>
@@ -1107,7 +1144,7 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="1:7" ht="15.75" thickBot="1">
+    <row r="23" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="3"/>
@@ -1116,7 +1153,7 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="1:7" ht="15.75" thickBot="1">
+    <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="3"/>
@@ -1125,7 +1162,7 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="1:7" ht="15.75" thickBot="1">
+    <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="3"/>
@@ -1134,7 +1171,7 @@
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="1:7" ht="15.75" thickBot="1">
+    <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="3"/>
@@ -1143,7 +1180,7 @@
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
     </row>
-    <row r="28" spans="1:7" ht="27.75">
+    <row r="28" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="8" t="s">
         <v>46</v>
       </c>
@@ -1152,7 +1189,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>47</v>
       </c>
@@ -1177,7 +1214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>48</v>
       </c>
@@ -1202,7 +1239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="10" t="s">
         <v>49</v>
       </c>
@@ -1210,7 +1247,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="79.5" customHeight="1">
+    <row r="34" spans="1:7" ht="79.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B34" s="11" t="s">
         <v>51</v>
       </c>
@@ -1220,7 +1257,7 @@
       <c r="F34" s="11"/>
       <c r="G34" s="11"/>
     </row>
-    <row r="35" spans="1:7" ht="47.25" customHeight="1">
+    <row r="35" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B35" s="11" t="s">
         <v>52</v>
       </c>
@@ -1230,7 +1267,7 @@
       <c r="F35" s="11"/>
       <c r="G35" s="11"/>
     </row>
-    <row r="36" spans="1:7" ht="44.25" customHeight="1">
+    <row r="36" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B36" s="11" t="s">
         <v>53</v>
       </c>
@@ -1240,7 +1277,7 @@
       <c r="F36" s="11"/>
       <c r="G36" s="11"/>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="D39" s="9"/>
     </row>
   </sheetData>
@@ -1284,12 +1321,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FC6F382-02E1-40C2-A4CE-CF742186EEF1}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="101.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E3" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1300,7 +1353,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1312,9 +1365,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -1330,7 +1383,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1342,22 +1395,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010099E9797445E2EA4280A45CB90FD95CBD" ma:contentTypeVersion="7" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="b362696dc43ecf0429c4c65f28c02171">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ba0fee18-8f7d-444d-be37-1e56d133d327" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="79fc1cf0b24a9b8e3e12f8f8264ba269" ns2:_="">
     <xsd:import namespace="ba0fee18-8f7d-444d-be37-1e56d133d327"/>
@@ -1519,6 +1563,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1526,13 +1579,36 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F4B272D-551A-4AF9-B220-C688C9745ED1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC0DDDC5-E50E-4F26-8594-4A1786F565B7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ba0fee18-8f7d-444d-be37-1e56d133d327"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC0DDDC5-E50E-4F26-8594-4A1786F565B7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F4B272D-551A-4AF9-B220-C688C9745ED1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D0D844A-E87E-42E2-B155-132CABE67861}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D0D844A-E87E-42E2-B155-132CABE67861}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>